<commit_message>
Add function for the output of the model
</commit_message>
<xml_diff>
--- a/Data(1).xlsx
+++ b/Data(1).xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Javi\Investigación\Publicaciones en preparación\Turnos_AECID\Caso de estudio Turquía\Gurobipy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C8F284-5250-4F53-BD83-E65984BE87D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C3E336-EA68-452D-B45A-AAB1A0A67E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="2" activeTab="4" xr2:uid="{04256E5A-9FC3-4ED9-8234-05D2531DDDEE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{04256E5A-9FC3-4ED9-8234-05D2531DDDEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Prices" sheetId="2" r:id="rId2"/>
-    <sheet name="Demand" sheetId="5" r:id="rId3"/>
-    <sheet name="HealthProfiles" sheetId="3" r:id="rId4"/>
-    <sheet name="Availability" sheetId="4" r:id="rId5"/>
+    <sheet name="Charter" sheetId="7" r:id="rId3"/>
+    <sheet name="Demand" sheetId="5" r:id="rId4"/>
+    <sheet name="HealthProfiles" sheetId="3" r:id="rId5"/>
+    <sheet name="Availability" sheetId="4" r:id="rId6"/>
+    <sheet name="Weights" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>N periods</t>
   </si>
@@ -54,12 +56,6 @@
     <t>Return</t>
   </si>
   <si>
-    <t>Profile</t>
-  </si>
-  <si>
-    <t>N. People</t>
-  </si>
-  <si>
     <t>Tperiod</t>
   </si>
   <si>
@@ -73,6 +69,111 @@
   </si>
   <si>
     <t>Max periods</t>
+  </si>
+  <si>
+    <t>Profile|Period</t>
+  </si>
+  <si>
+    <t>Person | Profile</t>
+  </si>
+  <si>
+    <t>Person | Period</t>
+  </si>
+  <si>
+    <t>Min periods</t>
+  </si>
+  <si>
+    <t>Chartered 1</t>
+  </si>
+  <si>
+    <t>Number chartered</t>
+  </si>
+  <si>
+    <t>Chartered 2</t>
+  </si>
+  <si>
+    <t>Min Cap</t>
+  </si>
+  <si>
+    <t>Max Cap</t>
+  </si>
+  <si>
+    <t>W1</t>
+  </si>
+  <si>
+    <t>W2</t>
+  </si>
+  <si>
+    <t>W3</t>
+  </si>
+  <si>
+    <t>ww1</t>
+  </si>
+  <si>
+    <t>ww2</t>
+  </si>
+  <si>
+    <t>weight for cost</t>
+  </si>
+  <si>
+    <t>weight for infeasibility</t>
+  </si>
+  <si>
+    <t>weight for second objective</t>
+  </si>
+  <si>
+    <t>weight for regular flights</t>
+  </si>
+  <si>
+    <t>weight for chartered flights</t>
+  </si>
+  <si>
+    <t>ww3</t>
+  </si>
+  <si>
+    <t>ww4</t>
+  </si>
+  <si>
+    <t>weight for number of roles</t>
+  </si>
+  <si>
+    <t>weight for availability</t>
+  </si>
+  <si>
+    <t>Nurse</t>
+  </si>
+  <si>
+    <t>Anaesthetist</t>
+  </si>
+  <si>
+    <t>Surgeon</t>
+  </si>
+  <si>
+    <t>Paediatrician</t>
+  </si>
+  <si>
+    <t>Gynaecologist</t>
+  </si>
+  <si>
+    <t>Family doctor</t>
+  </si>
+  <si>
+    <t>NS</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>GY</t>
+  </si>
+  <si>
+    <t>FD</t>
   </si>
 </sst>
 </file>
@@ -108,8 +209,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,15 +526,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22DD53F-E6F1-4891-883C-B1C2BD5A9532}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -461,26 +562,42 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
         <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -492,18 +609,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD52FD11-6791-44F4-B991-07326E921E19}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -581,70 +701,125 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4881C639-351C-43B8-B9DD-234D25D73EF1}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1D44DA-F94A-43B8-B9CC-776CC5E8D5A1}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C2" s="1">
+        <v>200000</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C3" s="1">
+        <v>200000</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="F3" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="B4" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C4" s="1">
+        <v>200000</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="B5" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C5" s="1">
+        <v>200000</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="B6" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>200000</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
+      <c r="B7" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C7" s="1">
+        <v>200000</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -652,19 +827,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF0EBB9-93AB-45CE-A86E-619D9EDDBA5E}">
-  <dimension ref="A1:G19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4881C639-351C-43B8-B9DD-234D25D73EF1}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="7" width="6.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="5.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
       <c r="B1">
         <v>1</v>
       </c>
@@ -689,22 +866,22 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -712,19 +889,19 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -735,19 +912,19 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -758,22 +935,22 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -781,22 +958,22 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -804,298 +981,22 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1104,19 +1005,502 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B57DF47-718C-4F4A-9599-E90E895B861B}">
-  <dimension ref="A1:G19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF0EBB9-93AB-45CE-A86E-619D9EDDBA5E}">
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B57DF47-718C-4F4A-9599-E90E895B861B}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="6.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
       <c r="B1">
         <v>1</v>
       </c>
@@ -1548,6 +1932,101 @@
       </c>
       <c r="G19">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E0CB66-6B98-4B27-8B97-D638EB39060C}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>99999999999</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>